<commit_message>
arreglando correcciones de flores de mis pantallas
</commit_message>
<xml_diff>
--- a/backend/src/tmp/Lista de participantes.xlsx
+++ b/backend/src/tmp/Lista de participantes.xlsx
@@ -11,12 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>Diego</t>
-  </si>
-  <si>
-    <t>Veramendi Malpartida</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>Diego + participante.apellidos</t>
   </si>
   <si>
     <t>v.dvm.dvm@gmail.com</t>
@@ -25,10 +22,7 @@
     <t>Líder</t>
   </si>
   <si>
-    <t>BRUCE ANTHONY</t>
-  </si>
-  <si>
-    <t>ESTRADA MELGAREJO</t>
+    <t>BRUCE ANTHONY + participante.apellidos</t>
   </si>
   <si>
     <t>a20203298@pucp.edu.pe</t>
@@ -37,19 +31,13 @@
     <t>Miembro</t>
   </si>
   <si>
-    <t>GABRIEL OMAR</t>
-  </si>
-  <si>
-    <t>DURAN RUIZ</t>
+    <t>GABRIEL OMAR + participante.apellidos</t>
   </si>
   <si>
     <t>a20203371@pucp.edu.pe</t>
   </si>
   <si>
-    <t>CHRISTIAN SEBASTIAN</t>
-  </si>
-  <si>
-    <t>CHIRA MALLQUI</t>
+    <t>CHRISTIAN SEBASTIAN + participante.apellidos</t>
   </si>
   <si>
     <t>s.chira@pucp.edu.pe</t>
@@ -429,16 +417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="1" max="1" width="46" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,50 +435,38 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>